<commit_message>
Updated OT with auto excel
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Milk/32th_Milk/Results/OTResults.xlsx
+++ b/P3/Results/Data/Milk/32th_Milk/Results/OTResults.xlsx
@@ -412,25 +412,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
-    <col width="28" customWidth="1" min="2" max="2"/>
-    <col width="27" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
-    <col width="29" customWidth="1" min="7" max="7"/>
-    <col width="26" customWidth="1" min="8" max="8"/>
-    <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="28" customWidth="1" min="10" max="10"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -455,32 +443,62 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Psnr Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Psnr Reference diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>MBE Ground diff Reference</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>MBE Ground diff Enhanced</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>MBE Reference diff Enhanced</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>MBE Reference diff Dehazed</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
         <is>
           <t>AG Ground diff Reference</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>AG Ground diff Enhanced</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>AG Reference diff Enhanced</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>AG Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>AG Reference diff Dehazed</t>
         </is>
       </c>
     </row>
@@ -500,22 +518,40 @@
         <v>6.14</v>
       </c>
       <c r="E2" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.21</v>
+      </c>
+      <c r="G2" t="n">
         <v>-97.22</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>-2.79</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>94.43000000000001</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
+        <v>-25.59</v>
+      </c>
+      <c r="K2" t="n">
+        <v>71.63</v>
+      </c>
+      <c r="L2" t="n">
         <v>3.38</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>-0.78</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>-4.16</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-6.93</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-10.31</v>
       </c>
     </row>
     <row r="3">
@@ -534,22 +570,40 @@
         <v>6.11</v>
       </c>
       <c r="E3" t="n">
+        <v>9.890000000000001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.17</v>
+      </c>
+      <c r="G3" t="n">
         <v>-97.56999999999999</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>-2.79</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>94.78</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
+        <v>-26.19</v>
+      </c>
+      <c r="K3" t="n">
+        <v>71.38</v>
+      </c>
+      <c r="L3" t="n">
         <v>3.38</v>
       </c>
-      <c r="I3" t="n">
+      <c r="M3" t="n">
         <v>-0.72</v>
       </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>-4.1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-6.92</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-10.3</v>
       </c>
     </row>
     <row r="4">
@@ -568,22 +622,40 @@
         <v>11.3</v>
       </c>
       <c r="E4" t="n">
+        <v>14.81</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="G4" t="n">
         <v>-46.76</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>-4.04</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>42.71</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
+        <v>9.06</v>
+      </c>
+      <c r="K4" t="n">
+        <v>55.81</v>
+      </c>
+      <c r="L4" t="n">
         <v>3.89</v>
       </c>
-      <c r="I4" t="n">
+      <c r="M4" t="n">
         <v>-6.17</v>
       </c>
-      <c r="J4" t="n">
+      <c r="N4" t="n">
         <v>-10.06</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.79</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-4.68</v>
       </c>
     </row>
     <row r="5">
@@ -602,158 +674,276 @@
         <v>11.32</v>
       </c>
       <c r="E5" t="n">
+        <v>14.88</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="G5" t="n">
         <v>-46.39</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>-4.1</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>42.29</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
+        <v>9.24</v>
+      </c>
+      <c r="K5" t="n">
+        <v>55.63</v>
+      </c>
+      <c r="L5" t="n">
         <v>3.92</v>
       </c>
-      <c r="I5" t="n">
+      <c r="M5" t="n">
         <v>-6.24</v>
       </c>
-      <c r="J5" t="n">
+      <c r="N5" t="n">
         <v>-10.16</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-0.74</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-4.66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Left_Side_20241611_121625.png</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4.17</v>
-      </c>
-      <c r="C6" t="n">
-        <v>14.64</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5.17</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-127.36</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-11.48</v>
-      </c>
-      <c r="G6" t="n">
-        <v>115.88</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-0.57</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-3.87</v>
+          <t>InFront_Camera_20241611_121413.png</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Left_Side_20241611_121631.png</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4.18</v>
-      </c>
-      <c r="C7" t="n">
-        <v>14.63</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-127.05</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-11.73</v>
-      </c>
-      <c r="G7" t="n">
-        <v>115.32</v>
-      </c>
-      <c r="H7" t="n">
-        <v>3.29</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.5600000000000001</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-3.85</v>
+          <t>InFront_Camera_20241611_121424.png</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Right_Side_20241611_121508.png</t>
+          <t>Left_Side_20241611_121625.png</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.57</v>
+        <v>4.17</v>
       </c>
       <c r="C8" t="n">
-        <v>14.95</v>
+        <v>14.64</v>
       </c>
       <c r="D8" t="n">
-        <v>5.32</v>
+        <v>5.17</v>
       </c>
       <c r="E8" t="n">
-        <v>-117.91</v>
+        <v>6.38</v>
       </c>
       <c r="F8" t="n">
-        <v>-6.27</v>
+        <v>3.81</v>
       </c>
       <c r="G8" t="n">
-        <v>111.65</v>
+        <v>-127.36</v>
       </c>
       <c r="H8" t="n">
-        <v>3.33</v>
+        <v>-11.48</v>
       </c>
       <c r="I8" t="n">
-        <v>0.37</v>
+        <v>115.88</v>
       </c>
       <c r="J8" t="n">
-        <v>-2.96</v>
+        <v>-61.65</v>
+      </c>
+      <c r="K8" t="n">
+        <v>65.70999999999999</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-0.57</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-3.87</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-5.14</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-8.44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Left_Side_20241611_121631.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="C9" t="n">
+        <v>14.63</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6.39</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-127.05</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-11.73</v>
+      </c>
+      <c r="I9" t="n">
+        <v>115.32</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-61.36</v>
+      </c>
+      <c r="K9" t="n">
+        <v>65.69</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-0.5600000000000001</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-3.85</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-5.11</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-8.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Right_Side_20241611_121508.png</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-117.91</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-6.27</v>
+      </c>
+      <c r="I10" t="n">
+        <v>111.65</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-52.37</v>
+      </c>
+      <c r="K10" t="n">
+        <v>65.54000000000001</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-2.96</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-4.48</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-7.81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Right_Side_20241611_121514.png</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B11" t="n">
         <v>4.57</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C11" t="n">
         <v>14.95</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D11" t="n">
         <v>5.35</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E11" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="G11" t="n">
         <v>-117.93</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H11" t="n">
         <v>-6.44</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I11" t="n">
         <v>111.49</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J11" t="n">
+        <v>-52.42</v>
+      </c>
+      <c r="K11" t="n">
+        <v>65.51000000000001</v>
+      </c>
+      <c r="L11" t="n">
         <v>3.32</v>
       </c>
-      <c r="I9" t="n">
+      <c r="M11" t="n">
         <v>0.32</v>
       </c>
-      <c r="J9" t="n">
+      <c r="N11" t="n">
         <v>-3</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-4.49</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-7.81</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Top_Down_20241611_121548.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Top_Down_20241611_121554.png</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>